<commit_message>
just updated important staffs
</commit_message>
<xml_diff>
--- a/SOFTWARE ENGINEERING/PROJECT/PROJECT REPORT/FINAL/Project_Timeline_group-1.xlsx
+++ b/SOFTWARE ENGINEERING/PROJECT/PROJECT REPORT/FINAL/Project_Timeline_group-1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SUMMER 23-24\SOFTWARE ENGINEERING\PROJECT\PROJECT REPORT\FINAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93C45C8-290F-48EE-9730-EFFEE2CC8742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8A7B3E-D421-4D57-95FF-275879514F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3B348EBE-DC41-41A9-813F-2952E0E64B8E}"/>
   </bookViews>
@@ -551,45 +551,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
@@ -604,28 +565,67 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1174,10 +1174,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41690466-6491-4B6C-8D72-841CDB06DEFA}">
-  <dimension ref="A1:AD15"/>
+  <dimension ref="A1:AC16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,175 +1205,175 @@
     <col min="27" max="29" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17"/>
-      <c r="B1" s="29">
+    <row r="1" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="36"/>
+      <c r="B1" s="16">
         <v>1</v>
       </c>
-      <c r="C1" s="30">
+      <c r="C1" s="17">
         <v>2</v>
       </c>
-      <c r="D1" s="23">
+      <c r="D1" s="10">
         <v>3</v>
       </c>
-      <c r="E1" s="23">
+      <c r="E1" s="10">
         <v>4</v>
       </c>
-      <c r="F1" s="23">
+      <c r="F1" s="10">
         <v>5</v>
       </c>
-      <c r="G1" s="23">
+      <c r="G1" s="10">
         <v>6</v>
       </c>
-      <c r="H1" s="23">
+      <c r="H1" s="10">
         <v>7</v>
       </c>
-      <c r="I1" s="23">
+      <c r="I1" s="10">
         <v>8</v>
       </c>
-      <c r="J1" s="23">
+      <c r="J1" s="10">
         <v>9</v>
       </c>
-      <c r="K1" s="23">
+      <c r="K1" s="10">
         <v>10</v>
       </c>
-      <c r="L1" s="23">
+      <c r="L1" s="10">
         <v>11</v>
       </c>
-      <c r="M1" s="23">
+      <c r="M1" s="10">
         <v>12</v>
       </c>
-      <c r="N1" s="23">
+      <c r="N1" s="10">
         <v>13</v>
       </c>
-      <c r="O1" s="23">
+      <c r="O1" s="10">
         <v>14</v>
       </c>
-      <c r="P1" s="23">
+      <c r="P1" s="10">
         <v>15</v>
       </c>
-      <c r="Q1" s="23">
+      <c r="Q1" s="10">
         <v>16</v>
       </c>
-      <c r="R1" s="23">
+      <c r="R1" s="10">
         <v>17</v>
       </c>
-      <c r="S1" s="23">
+      <c r="S1" s="10">
         <v>18</v>
       </c>
-      <c r="T1" s="23">
+      <c r="T1" s="10">
         <v>19</v>
       </c>
-      <c r="U1" s="23">
+      <c r="U1" s="10">
         <v>20</v>
       </c>
-      <c r="V1" s="23">
+      <c r="V1" s="10">
         <v>21</v>
       </c>
-      <c r="W1" s="23">
+      <c r="W1" s="10">
         <v>22</v>
       </c>
-      <c r="X1" s="23">
+      <c r="X1" s="10">
         <v>23</v>
       </c>
-      <c r="Y1" s="23">
+      <c r="Y1" s="10">
         <v>24</v>
       </c>
-      <c r="Z1" s="23">
+      <c r="Z1" s="10">
         <v>25</v>
       </c>
-      <c r="AA1" s="23">
+      <c r="AA1" s="10">
         <v>26</v>
       </c>
-      <c r="AB1" s="23">
+      <c r="AB1" s="10">
         <v>27</v>
       </c>
-      <c r="AC1" s="24">
+      <c r="AC1" s="11">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="37"/>
+      <c r="B2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="14" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="8" t="s">
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="34"/>
+      <c r="AA2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="10"/>
+      <c r="AB2" s="28"/>
+      <c r="AC2" s="29"/>
     </row>
-    <row r="3" spans="1:30" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="14" t="s">
+    <row r="3" spans="1:29" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="38"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="14" t="s">
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="14" t="s">
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="14" t="s">
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="35"/>
+      <c r="V3" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15"/>
-      <c r="Z3" s="16"/>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="12"/>
-      <c r="AC3" s="13"/>
+      <c r="W3" s="34"/>
+      <c r="X3" s="34"/>
+      <c r="Y3" s="34"/>
+      <c r="Z3" s="35"/>
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="31"/>
+      <c r="AC3" s="32"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+    <row r="4" spans="1:29" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="34"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="5"/>
       <c r="E4" s="4"/>
       <c r="F4" s="2"/>
@@ -1399,17 +1399,17 @@
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
-      <c r="AC4" s="25"/>
+      <c r="AC4" s="12"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="37"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="23"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1432,10 +1432,10 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
-      <c r="AC5" s="27"/>
+      <c r="AC5" s="14"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1"/>
@@ -1443,32 +1443,32 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="38"/>
+      <c r="G6" s="19"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="39"/>
+      <c r="L6" s="20"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="39"/>
+      <c r="Q6" s="20"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
-      <c r="V6" s="39"/>
+      <c r="V6" s="20"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
-      <c r="AC6" s="27"/>
+      <c r="AC6" s="14"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1"/>
@@ -1477,31 +1477,31 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="39"/>
+      <c r="H7" s="20"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="39"/>
+      <c r="M7" s="20"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="39"/>
+      <c r="R7" s="20"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
-      <c r="W7" s="39"/>
+      <c r="W7" s="20"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
-      <c r="AC7" s="27"/>
+      <c r="AC7" s="14"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1"/>
@@ -1511,30 +1511,30 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="37"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="23"/>
       <c r="K8" s="3"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="37"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="23"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
-      <c r="S8" s="35"/>
-      <c r="T8" s="37"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="23"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
-      <c r="X8" s="35"/>
-      <c r="Y8" s="37"/>
+      <c r="X8" s="22"/>
+      <c r="Y8" s="23"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
-      <c r="AC8" s="27"/>
+      <c r="AC8" s="14"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1"/>
@@ -1546,28 +1546,28 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="38"/>
+      <c r="K9" s="19"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="39"/>
+      <c r="P9" s="20"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
-      <c r="U9" s="39"/>
+      <c r="U9" s="20"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
-      <c r="Z9" s="39"/>
+      <c r="Z9" s="20"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
-      <c r="AC9" s="27"/>
+      <c r="AC9" s="14"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1"/>
@@ -1595,63 +1595,71 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
-      <c r="AA10" s="35"/>
-      <c r="AB10" s="37"/>
-      <c r="AC10" s="27"/>
+      <c r="AA10" s="22"/>
+      <c r="AB10" s="23"/>
+      <c r="AC10" s="14"/>
     </row>
-    <row r="11" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+    <row r="11" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="21"/>
-      <c r="X11" s="21"/>
-      <c r="Y11" s="21"/>
-      <c r="Z11" s="21"/>
-      <c r="AA11" s="21"/>
-      <c r="AB11" s="21"/>
-      <c r="AC11" s="40"/>
-      <c r="AD11" s="31"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="21"/>
     </row>
-    <row r="12" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
-      <c r="AD12" s="31"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="C14" s="31"/>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="C15" s="31"/>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="X8:Y8"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="S8:T8"/>
     <mergeCell ref="AA2:AC3"/>
     <mergeCell ref="V3:Z3"/>
     <mergeCell ref="A1:A3"/>
@@ -1660,6 +1668,13 @@
     <mergeCell ref="L3:P3"/>
     <mergeCell ref="Q3:U3"/>
     <mergeCell ref="G2:Z2"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="X8:Y8"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="S8:T8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>